<commit_message>
fixed doc and const var where memory for vm was invalid
</commit_message>
<xml_diff>
--- a/docs/vm_sizes.xlsx
+++ b/docs/vm_sizes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharpiro\Desktop\temp\az-cli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitbase\Azure\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -60,7 +60,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,8 +96,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,109 +416,110 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>4.46</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8.93</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>8.93</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>17.86</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>17.86</v>
-      </c>
-      <c r="C4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>34.97</v>
+      </c>
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D5" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>69.94</v>
+      </c>
+      <c r="C6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>34.97</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
+      <c r="D6" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>139.87</v>
+      </c>
+      <c r="C7" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>69.94</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>139.87</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>32</v>
       </c>
     </row>

</xml_diff>